<commit_message>
Testing commit. Changed the map a bit.
</commit_message>
<xml_diff>
--- a/Heart_Of_Virtue/heart_of_virtue/resources/map_editor.xlsx
+++ b/Heart_Of_Virtue/heart_of_virtue/resources/map_editor.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="6">
   <si>
     <t>StartingRoom</t>
   </si>
@@ -378,7 +378,7 @@
   <dimension ref="B3:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -387,8 +387,8 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F3" s="1" t="s">
-        <v>4</v>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>5</v>
@@ -417,6 +417,9 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Finished up the player's inventory menu.
</commit_message>
<xml_diff>
--- a/Heart_Of_Virtue/heart_of_virtue/resources/map_editor.xlsx
+++ b/Heart_Of_Virtue/heart_of_virtue/resources/map_editor.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="5">
   <si>
     <t>StartingRoom</t>
   </si>
@@ -25,9 +25,6 @@
   </si>
   <si>
     <t>GiantSpiderRoom</t>
-  </si>
-  <si>
-    <t>FindDaggerRoom</t>
   </si>
   <si>
     <t>LeaveCaveRoom</t>
@@ -378,7 +375,7 @@
   <dimension ref="B3:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -391,7 +388,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -405,7 +402,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -413,18 +410,18 @@
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -440,11 +437,8 @@
       <c r="E7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -452,7 +446,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up map generation
</commit_message>
<xml_diff>
--- a/Heart_Of_Virtue/heart_of_virtue/resources/map_editor.xlsx
+++ b/Heart_Of_Virtue/heart_of_virtue/resources/map_editor.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
   <si>
     <t>StartingRoom</t>
   </si>
@@ -24,13 +24,16 @@
     <t>EmptyCavePath</t>
   </si>
   <si>
-    <t>GiantSpiderRoom</t>
-  </si>
-  <si>
     <t>LeaveCaveRoom</t>
   </si>
   <si>
     <t>Boundary</t>
+  </si>
+  <si>
+    <t>Syntax: tile_name, other attributes</t>
+  </si>
+  <si>
+    <t>Other attributes are added with syntax "&lt;object name&gt;:&lt;quantity&gt;"</t>
   </si>
 </sst>
 </file>
@@ -66,10 +69,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -372,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B3" sqref="B3:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -383,50 +392,58 @@
     <col min="1" max="16384" width="17.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>1</v>
@@ -438,15 +455,15 @@
         <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work on map generations, enemies, etc.
</commit_message>
<xml_diff>
--- a/Heart_Of_Virtue/heart_of_virtue/resources/map_editor.xlsx
+++ b/Heart_Of_Virtue/heart_of_virtue/resources/map_editor.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="4">
   <si>
     <t>StartingRoom</t>
   </si>
@@ -28,12 +28,6 @@
   </si>
   <si>
     <t>Boundary</t>
-  </si>
-  <si>
-    <t>Syntax: tile_name, other attributes</t>
-  </si>
-  <si>
-    <t>Other attributes are added with syntax "&lt;object name&gt;:&lt;quantity&gt;"</t>
   </si>
 </sst>
 </file>
@@ -69,16 +63,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -381,48 +369,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:H8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="17.42578125" style="1"/>
+    <col min="1" max="1" width="4" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="17.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="1">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="H4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
@@ -430,40 +472,70 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>1</v>
+    <row r="7" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>3</v>
+    <row r="8" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Cleaned up Tile_Description parsing. Tile_Description parameter set needs to end with '~' instead of a '.' for parsing purposes. This fixes the bug where the final period was dropped because of the 'string'.split() function. - Improved the map interface so that it's monospaced (the big characters threw the monospacing out of whack.)  - Added tile discovery to the map, where known exits appear as '?'  - Added features to set a room's map symbol. Defaults are set in the tiles module under each child class.
</commit_message>
<xml_diff>
--- a/Heart_Of_Virtue/heart_of_virtue/resources/map_editor.xlsx
+++ b/Heart_Of_Virtue/heart_of_virtue/resources/map_editor.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
   <si>
     <t>StartingRoom</t>
   </si>
@@ -42,10 +42,13 @@
     <t>EmptyCave|@Wooden_Chest.1.#Gold:12</t>
   </si>
   <si>
-    <t xml:space="preserve">EmptyCave|@Hidden_Wall_Switch.1.h0|!Block.east|!Story.0.r|@Tile_Description.1.The wall here feels warmer than the rest of the cavern. There are scuff marks on the floor that stop abruptly where the wall and floor meet. Jean can hear the muffled sound of flowing water. </t>
-  </si>
-  <si>
-    <t>EmptyCave|!Story.1.r.p</t>
+    <t>BlankTile|@Tile_Description.1.A long rock ledge juts out from the opening to the west, crossing the chasm below and connecting to another rock wall to the east. The sunlight is blinding, with an open sky overhead. Far below, a river rushes beneath the ledge, spraying water in all directions as it crashes against the walls. The twittering of nearby birds can be heard. Banding to the east and west, a line of rock spires can be seen, including the two adjacent walls, all presumably connected by similar rock ledges. There's a warm breeze blowing mildly from the north~</t>
+  </si>
+  <si>
+    <t>BlankTile|@Wall_Switch.1.h0.!Story:0|!Block.east|@Tile_Description.1.The wall here feels warmer than the rest of the cavern. There are scuff marks on the floor that stop abruptly where the wall and floor meet. Jean can hear the muffled sound of flowing water~</t>
+  </si>
+  <si>
+    <t>BlankTile|!Block.east|@Tile_Description.1.The rock ledge continues to the east and terminates as it reaches the wall. From this vantage point, large mountains can be seen to the northwest, covered in white clouds at their crowns~|@Wall_Switch.1.!Story:1</t>
   </si>
 </sst>
 </file>
@@ -314,7 +317,19 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>&lt;classname&gt;.&lt;count&gt;.&lt;hidden [h(factor)] (leave blank for visible)&gt; - Also accepts arbitrary values like v0, which it passes as a list to param</a:t>
+            <a:t>&lt;classname&gt;.&lt;count&gt;.&lt;hidden [h(factor)] (leave blank for visible)&gt; - Also accepts arbitrary values like v0, which it passes as a list to param. For Tile_Descriptions,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> end with '~' instead of '.'</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1000">
             <a:effectLst/>
@@ -616,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -712,13 +727,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>2</v>
@@ -797,9 +812,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E4"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>